<commit_message>
Add browser version in test data
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E91401-FC1D-EA47-BBAA-2E443A89A3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D9FCC3-FE9F-1A44-851A-B18E57CA1A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>execute</t>
   </si>
@@ -51,9 +51,6 @@
     <t>browser</t>
   </si>
   <si>
-    <t>chrome</t>
-  </si>
-  <si>
     <t>YWRtaW4xMjM=</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t>testCaseName</t>
   </si>
   <si>
-    <t>safari</t>
-  </si>
-  <si>
     <t>To check whether the user can register successfully</t>
   </si>
   <si>
@@ -75,10 +69,13 @@
     <t>newTest</t>
   </si>
   <si>
-    <t>admin1</t>
-  </si>
-  <si>
-    <t>admin2</t>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>102.0</t>
   </si>
 </sst>
 </file>
@@ -466,7 +463,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -480,10 +477,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -514,10 +511,10 @@
     </row>
     <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
@@ -537,23 +534,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C2" sqref="C2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.1640625" customWidth="1"/>
-    <col min="2" max="3" width="18.1640625" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="29.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -562,13 +559,16 @@
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -576,16 +576,19 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -593,47 +596,56 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>12</v>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>